<commit_message>
Updated source for 3rd path of questions for Minfin
</commit_message>
<xml_diff>
--- a/data/minfin/3_questions.xlsx
+++ b/data/minfin/3_questions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
@@ -10,8 +10,8 @@
     <sheet name="questions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>question</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Государственная программа – это документ стратегического планирования, содержащий комплекс планируемых мероприятий и инструментов государственной политики, обеспечивающих достижение приоритетов и целей государственной политики в сфере социально-экономического развития и обеспечения национальной безопасности</t>
   </si>
   <si>
-    <t xml:space="preserve">Государственная программа – это документ стратегического планирования, содержащий комплекс планируемых мероприятий, взаимоувязанных по задачам, срокам осуществления, исполнителям и ресурсам, и инструментамов государственной политики, обеспечивающих в рамках реализации ключевых государственных функций достижение приоритетов и целей государственной политики в сфере социально-экономического развития и обеспечения национальной безопасности.
-Государственная программа может включать в себя подпрограммы, раскрывающие определенные направления развития или проблемную сферу.
-Государственная программа включает: титульный лист, паспорт государственной программы, паспорта подпрограмм, паспорта федеральных целевых программ, текстовую часть, приложения.
-</t>
-  </si>
-  <si>
     <t>Что, Такое, Государственная программа, Госпрограмма</t>
   </si>
   <si>
@@ -139,12 +133,6 @@
   </si>
   <si>
     <t>Государственные программы Российской Федерации включают  в себя подпрограммы, содержащие, ведомственные целевые программы и основные мероприятия органов государственной власти Российской Федерации</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Государственная программа включает федеральные целевые программы (в случае их наличия), реализуемые в соответствующей сфере социально - экономического развития или обеспечения национальной безопасности Российской Федерации, и подпрограммы, представляющие собой взаимоувязанные по целям, срокам и ресурсам мероприятия, выделенные исходя из масштаба и сложности задач, решаемых в рамках государственной программы, содержащие ведомственные целевые программы и основные мероприятия.
-Федеральная целевая программа может быть включена в состав только одной государственной программы. Допускается аналитическое (справочное) отражение в государственной программе: частей федеральных целевых программ; федеральных целевых программ, реализация которых направлена на достижение целей иных государственных программ.
-Государственная программа включает: титульный лист, паспорт государственной программы, паспорта подпрограмм, паспорта федеральных целевых программ, текстовую часть, приложения.
-</t>
   </si>
   <si>
     <t>3.7</t>
@@ -302,12 +290,43 @@
   <si>
     <t>Dinamika_Suverennie fondi.pdf</t>
   </si>
+  <si>
+    <t>Актуальная информация по исполнению государственных программ содержится на следующих информационных ресурсах в сети «Интернет»:
+- «Портал государственных программ»;
+- Раздел «Государственные программы» на сайте Правительства России;
+- Раздел «Расходы» - «Государственные программы» на Едином портале бюджетной системы «Электронный бюджет»</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Государственная программа – это документ стратегического планирования, содержащий комплекс планируемых мероприятий, взаимоувязанных по задачам, срокам осуществления, исполнителям и ресурсам, и инструментамам государственной политики, обеспечивающих в рамках реализации ключевых государственных функций достижение приоритетов и целей государственной политики в сфере социально-экономического развития и обеспечения национальной безопасности.
+Государственная программа включает в себя подпрограммы, направленные на достижение целей и решения задач государственной программы.
+Государственная программа включает: паспорт государственной программы, паспорта подпрограмм, паспорта федеральных целевых программ, текстовую часть, приложения.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Государственные программы субъекта Российской Федерации, муниципальные программы утверждаются соответственно высшим исполнительным органом государственной власти субъекта Российской Федерации, местной администрацией муниципального образования.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Государственная программа включает федеральные целевые программы (в случае их наличия), реализуемые в соответствующей сфере социально - экономического развития или обеспечения национальной безопасности Российской Федерации, и подпрограммы, представляющие собой взаимоувязанные по целям, срокам и ресурсам мероприятия, выделенные исходя из масштаба и сложности задач, решаемых в рамках государственной программы, содержащие ведомственные целевые программы и основные мероприятия.
+Федеральная целевая программа может быть включена в состав только одной государственной программы. Допускается аналитическое (справочное) отражение в государственной программе: частей федеральных целевых программ; федеральных целевых программ, реализация которых направлена на достижение целей иных государственных программ.
+Государственная программа содержит:
+- паспорт госпрограммы, паспорта подпрограмм, паспорта федеральных целевых программ (в случае наличия);
+- приоритеты и цели государственной политики и общие требования к политике субъектов Российской Федерации в соответствующей сфере;
+- перечень и характеристики основных мероприятий государственной программы и ведомственных целевых программ;
+- основные меры правового регулирования в соответствующей сфере;
+- перечень и сведения о целевых индикаторах и показателях государственной программы;
+- информацию по финансовому обеспечению государственной программы;
+- информацию по финансовому обеспечению государственной программы (в случае наличия);
+- правила предоставления субсидий из федерального бюджета бюджетам субъектов Российской Федерации в рамках государственной программы (в случае наличия);
+- план реализации государственной программы на очередной финансовый год и плановый период.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,7 +366,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -391,6 +410,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -707,27 +729,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="48" style="3" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="101.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="78.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="68.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -739,7 +761,7 @@
     <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -777,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="204.75">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -787,244 +809,253 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="141.75">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="186.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="94.5">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="78.75">
+      <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:12" ht="78.75">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="126" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="409.5">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="393.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    <row r="8" spans="1:12" s="8" customFormat="1" ht="126">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="B8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="141.75">
+      <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="8" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="126">
+      <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="378" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="236.25">
+      <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="63">
+      <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="94.5">
+      <c r="A13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="126" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="H13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:12" ht="315">
+      <c r="A14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="393.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="F14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>